<commit_message>
Updated r shiny feature and OR
</commit_message>
<xml_diff>
--- a/Development/Results/model.xlsx
+++ b/Development/Results/model.xlsx
@@ -98,61 +98,61 @@
     <t xml:space="preserve">25.2</t>
   </si>
   <si>
-    <t xml:space="preserve">BSKgezien=Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.686</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.289; 1.791]</t>
+    <t xml:space="preserve">CorrCa24u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.458</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.112; 17.271]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.426</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.121; 15.428]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BSKgezien - No:Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.479</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[2.906; 3.042]</t>
   </si>
   <si>
     <t xml:space="preserve">7.2</t>
   </si>
   <si>
-    <t xml:space="preserve">0.701</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.306; 1.755]</t>
+    <t xml:space="preserve">3.778</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.335; 7.648]</t>
   </si>
   <si>
     <t xml:space="preserve">8.9</t>
   </si>
   <si>
-    <t xml:space="preserve">CorrCa24u</t>
+    <t xml:space="preserve">Age_Years</t>
   </si>
   <si>
     <t xml:space="preserve">1.157</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.091; 14.113]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.265</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.028; 3.539]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age_Years</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.287</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.329; 0.344]</t>
+    <t xml:space="preserve">[0.456; 2.827]</t>
   </si>
   <si>
     <t xml:space="preserve">0.2</t>
   </si>
   <si>
-    <t xml:space="preserve">Sex=Male</t>
+    <t xml:space="preserve">Sex - Male:Female</t>
   </si>
   <si>
     <t xml:space="preserve">0.999</t>
@@ -164,7 +164,7 @@
     <t xml:space="preserve">0.0</t>
   </si>
   <si>
-    <t xml:space="preserve">surgery_type=total</t>
+    <t xml:space="preserve">surgery_type - completion:total</t>
   </si>
   <si>
     <t xml:space="preserve">1.484</t>
@@ -176,7 +176,7 @@
     <t xml:space="preserve">0.4</t>
   </si>
   <si>
-    <t xml:space="preserve">CHKD=Yes</t>
+    <t xml:space="preserve">CHKD - Yes:No</t>
   </si>
   <si>
     <t xml:space="preserve">1.379</t>

</xml_diff>

<commit_message>
First update of manuscript
</commit_message>
<xml_diff>
--- a/Development/Results/model.xlsx
+++ b/Development/Results/model.xlsx
@@ -50,19 +50,19 @@
     <t xml:space="preserve">Intercept</t>
   </si>
   <si>
-    <t xml:space="preserve">2.48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1.80; 3.42]</t>
+    <t xml:space="preserve">2.52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.82; 3.48]</t>
   </si>
   <si>
     <t xml:space="preserve"/>
   </si>
   <si>
-    <t xml:space="preserve">1.84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1.35; 2.51]</t>
+    <t xml:space="preserve">1.86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.36; 2.54]</t>
   </si>
   <si>
     <t xml:space="preserve">0.00</t>
@@ -77,18 +77,18 @@
     <t xml:space="preserve">1.08</t>
   </si>
   <si>
-    <t xml:space="preserve">[1.04; 1.12]</t>
+    <t xml:space="preserve">[1.05; 1.12]</t>
   </si>
   <si>
     <t xml:space="preserve">20.6</t>
   </si>
   <si>
-    <t xml:space="preserve">[1.05; 1.12]</t>
-  </si>
-  <si>
     <t xml:space="preserve">22.5</t>
   </si>
   <si>
+    <t xml:space="preserve">1.09</t>
+  </si>
+  <si>
     <t xml:space="preserve">28.3</t>
   </si>
   <si>
@@ -98,7 +98,7 @@
     <t xml:space="preserve">1.47</t>
   </si>
   <si>
-    <t xml:space="preserve">[1.13; 1.91]</t>
+    <t xml:space="preserve">[1.13; 1.92]</t>
   </si>
   <si>
     <t xml:space="preserve">8.1</t>
@@ -107,7 +107,7 @@
     <t xml:space="preserve">1.44</t>
   </si>
   <si>
-    <t xml:space="preserve">[1.11; 1.86]</t>
+    <t xml:space="preserve">[1.11; 1.87]</t>
   </si>
   <si>
     <t xml:space="preserve">7.8</t>
@@ -116,19 +116,19 @@
     <t xml:space="preserve">BSKgezien - No:Yes</t>
   </si>
   <si>
-    <t xml:space="preserve">3.64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1.46; 9.09]</t>
+    <t xml:space="preserve">3.67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.46; 9.23]</t>
   </si>
   <si>
     <t xml:space="preserve">7.7</t>
   </si>
   <si>
-    <t xml:space="preserve">3.90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1.62; 9.37]</t>
+    <t xml:space="preserve">3.94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.63; 9.53]</t>
   </si>
   <si>
     <t xml:space="preserve">9.3</t>
@@ -140,7 +140,7 @@
     <t xml:space="preserve">1.14</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.62; 2.10]</t>
+    <t xml:space="preserve">[0.61; 2.11]</t>
   </si>
   <si>
     <t xml:space="preserve">0.2</t>
@@ -152,7 +152,7 @@
     <t xml:space="preserve">0.95</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.45; 2.01]</t>
+    <t xml:space="preserve">[0.45; 2.02]</t>
   </si>
   <si>
     <t xml:space="preserve">0.0</t>
@@ -161,7 +161,7 @@
     <t xml:space="preserve">surgery_type - completion:total</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.44; 4.85]</t>
+    <t xml:space="preserve">[0.44; 4.91]</t>
   </si>
   <si>
     <t xml:space="preserve">0.4</t>
@@ -173,7 +173,7 @@
     <t xml:space="preserve">1.33</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.62; 2.85]</t>
+    <t xml:space="preserve">[0.61; 2.87]</t>
   </si>
   <si>
     <t xml:space="preserve">0.5</t>
@@ -194,7 +194,7 @@
     <t xml:space="preserve">0.85</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.81; 0.89]</t>
+    <t xml:space="preserve">[0.81; 0.90]</t>
   </si>
 </sst>
 </file>
@@ -622,19 +622,19 @@
         <v>20</v>
       </c>
       <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
         <v>24</v>
       </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" t="s">
-        <v>20</v>
-      </c>
       <c r="K3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L3" t="s">
         <v>25</v>

</xml_diff>